<commit_message>
atualizacao do arquivo com novo atributo
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>nome</t>
   </si>
@@ -44,6 +44,33 @@
   </si>
   <si>
     <t>4299999915</t>
+  </si>
+  <si>
+    <t>Nome 5</t>
+  </si>
+  <si>
+    <t>Nome 6</t>
+  </si>
+  <si>
+    <t>endereco</t>
+  </si>
+  <si>
+    <t>rua x</t>
+  </si>
+  <si>
+    <t>rua y</t>
+  </si>
+  <si>
+    <t>rua z</t>
+  </si>
+  <si>
+    <t>rua teste</t>
+  </si>
+  <si>
+    <t>rua nova</t>
+  </si>
+  <si>
+    <t>rua 123</t>
   </si>
 </sst>
 </file>
@@ -404,9 +431,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -414,44 +443,81 @@
     <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>4299999916</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>4299999917</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualizacao retirada de duas instancias
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>nome</t>
   </si>
@@ -22,18 +22,6 @@
     <t>telefone_completo</t>
   </si>
   <si>
-    <t>Nome 1</t>
-  </si>
-  <si>
-    <t>4299999912</t>
-  </si>
-  <si>
-    <t>Nome 2</t>
-  </si>
-  <si>
-    <t>4299999913</t>
-  </si>
-  <si>
     <t>Nome 3</t>
   </si>
   <si>
@@ -53,12 +41,6 @@
   </si>
   <si>
     <t>endereco</t>
-  </si>
-  <si>
-    <t>rua x</t>
-  </si>
-  <si>
-    <t>rua y</t>
   </si>
   <si>
     <t>rua z</t>
@@ -434,7 +416,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,73 +433,51 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>4299999916</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>4299999917</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>